<commit_message>
Lots of fixes, some nerfs and clean up
</commit_message>
<xml_diff>
--- a/resources/data-imports/Affixes/skill_res_reduc_plus_devouring.xlsx
+++ b/resources/data-imports/Affixes/skill_res_reduc_plus_devouring.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Affixes" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Affixes" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -389,7 +389,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -405,6 +405,112 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -412,15 +518,15 @@
   </sheetPr>
   <dimension ref="A1:AT25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AI1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AS33" activeCellId="0" sqref="AS33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AK17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AT25" activeCellId="0" sqref="AT25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="32.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="32.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14"/>
@@ -452,7 +558,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="43" style="1" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="24.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="0" width="16.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="16.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -591,7 +697,7 @@
       <c r="AS1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="0" t="s">
+      <c r="AT1" s="1" t="s">
         <v>45</v>
       </c>
     </row>
@@ -686,7 +792,7 @@
       <c r="AS2" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="AT2" s="0" t="n">
+      <c r="AT2" s="1" t="n">
         <v>3</v>
       </c>
     </row>
@@ -781,7 +887,7 @@
       <c r="AS3" s="1" t="n">
         <v>0.0122</v>
       </c>
-      <c r="AT3" s="0" t="n">
+      <c r="AT3" s="1" t="n">
         <v>3</v>
       </c>
     </row>
@@ -876,7 +982,7 @@
       <c r="AS4" s="1" t="n">
         <v>0.0149</v>
       </c>
-      <c r="AT4" s="0" t="n">
+      <c r="AT4" s="1" t="n">
         <v>3</v>
       </c>
     </row>
@@ -971,7 +1077,7 @@
       <c r="AS5" s="1" t="n">
         <v>0.0182</v>
       </c>
-      <c r="AT5" s="0" t="n">
+      <c r="AT5" s="1" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1066,7 +1172,7 @@
       <c r="AS6" s="1" t="n">
         <v>0.0223</v>
       </c>
-      <c r="AT6" s="0" t="n">
+      <c r="AT6" s="1" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1161,7 +1267,7 @@
       <c r="AS7" s="1" t="n">
         <v>0.0272</v>
       </c>
-      <c r="AT7" s="0" t="n">
+      <c r="AT7" s="1" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1256,7 +1362,7 @@
       <c r="AS8" s="1" t="n">
         <v>0.0332</v>
       </c>
-      <c r="AT8" s="0" t="n">
+      <c r="AT8" s="1" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1351,11 +1457,11 @@
       <c r="AS9" s="1" t="n">
         <v>0.0406</v>
       </c>
-      <c r="AT9" s="0" t="n">
+      <c r="AT9" s="1" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
@@ -1446,7 +1552,7 @@
       <c r="AS10" s="1" t="n">
         <v>0.0496</v>
       </c>
-      <c r="AT10" s="0" t="n">
+      <c r="AT10" s="1" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1541,7 +1647,7 @@
       <c r="AS11" s="1" t="n">
         <v>0.0606</v>
       </c>
-      <c r="AT11" s="0" t="n">
+      <c r="AT11" s="1" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1636,7 +1742,7 @@
       <c r="AS12" s="1" t="n">
         <v>0.0741</v>
       </c>
-      <c r="AT12" s="0" t="n">
+      <c r="AT12" s="1" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1731,7 +1837,7 @@
       <c r="AS13" s="1" t="n">
         <v>0.0905</v>
       </c>
-      <c r="AT13" s="0" t="n">
+      <c r="AT13" s="1" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1826,11 +1932,11 @@
       <c r="AS14" s="1" t="n">
         <v>0.1248</v>
       </c>
-      <c r="AT14" s="0" t="n">
+      <c r="AT14" s="1" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
@@ -1921,7 +2027,7 @@
       <c r="AS15" s="1" t="n">
         <v>0.1541</v>
       </c>
-      <c r="AT15" s="0" t="n">
+      <c r="AT15" s="1" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2016,7 +2122,7 @@
       <c r="AS16" s="1" t="n">
         <v>0.1901</v>
       </c>
-      <c r="AT16" s="0" t="n">
+      <c r="AT16" s="1" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2111,7 +2217,7 @@
       <c r="AS17" s="1" t="n">
         <v>0.2347</v>
       </c>
-      <c r="AT17" s="0" t="n">
+      <c r="AT17" s="1" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2206,7 +2312,7 @@
       <c r="AS18" s="1" t="n">
         <v>0.2896</v>
       </c>
-      <c r="AT18" s="0" t="n">
+      <c r="AT18" s="1" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2301,7 +2407,7 @@
       <c r="AS19" s="1" t="n">
         <v>0.3574</v>
       </c>
-      <c r="AT19" s="0" t="n">
+      <c r="AT19" s="1" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2396,7 +2502,7 @@
       <c r="AS20" s="1" t="n">
         <v>0.4411</v>
       </c>
-      <c r="AT20" s="0" t="n">
+      <c r="AT20" s="1" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2491,7 +2597,7 @@
       <c r="AS21" s="1" t="n">
         <v>0.5444</v>
       </c>
-      <c r="AT21" s="0" t="n">
+      <c r="AT21" s="1" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2586,7 +2692,7 @@
       <c r="AS22" s="1" t="n">
         <v>0.6719</v>
       </c>
-      <c r="AT22" s="0" t="n">
+      <c r="AT22" s="1" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2681,7 +2787,7 @@
       <c r="AS23" s="1" t="n">
         <v>0.802</v>
       </c>
-      <c r="AT23" s="0" t="n">
+      <c r="AT23" s="1" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2776,7 +2882,7 @@
       <c r="AS24" s="1" t="n">
         <v>0.804</v>
       </c>
-      <c r="AT24" s="0" t="n">
+      <c r="AT24" s="1" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2863,15 +2969,15 @@
         <v>0</v>
       </c>
       <c r="AQ25" s="1" t="n">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="AR25" s="1" t="n">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="AS25" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT25" s="0" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="AT25" s="1" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>